<commit_message>
Commit All Complate Task demand & time
</commit_message>
<xml_diff>
--- a/cypress/fixtures/loginData3.xlsx
+++ b/cypress/fixtures/loginData3.xlsx
@@ -1,32 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\project\cypress\BankUltimus_Automation\cypress\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{331B6003-181E-48C2-9558-84FDA2CA105F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D48FB17-A5D4-4514-9C5A-DCBCF599375C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="5" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="888" firstSheet="7" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="EmployeeDetails" sheetId="15" r:id="rId2"/>
-    <sheet name="MenuSearch" sheetId="2" r:id="rId3"/>
-    <sheet name="DefineCreditLine" sheetId="13" r:id="rId4"/>
+    <sheet name="MenuSearch" sheetId="2" r:id="rId2"/>
+    <sheet name="DDAccOpen" sheetId="3" r:id="rId3"/>
+    <sheet name="SDAccOpen" sheetId="12" r:id="rId4"/>
     <sheet name="TDAccOpen" sheetId="11" r:id="rId5"/>
-    <sheet name="FinProposalRegister" sheetId="14" r:id="rId6"/>
-    <sheet name="DDAccOpen" sheetId="3" r:id="rId7"/>
-    <sheet name="SDAccOpen" sheetId="12" r:id="rId8"/>
-    <sheet name="NftAuth" sheetId="4" r:id="rId9"/>
-    <sheet name="DDTrans" sheetId="7" r:id="rId10"/>
-    <sheet name="TransAuth" sheetId="8" r:id="rId11"/>
-    <sheet name="AccountInquary" sheetId="10" r:id="rId12"/>
+    <sheet name="NftAuth" sheetId="4" r:id="rId6"/>
+    <sheet name="DDTrans" sheetId="7" r:id="rId7"/>
+    <sheet name="SDTrans" sheetId="16" r:id="rId8"/>
+    <sheet name="TDTrans" sheetId="17" r:id="rId9"/>
+    <sheet name="TransAuth" sheetId="8" r:id="rId10"/>
+    <sheet name="AccountInquary" sheetId="10" r:id="rId11"/>
+    <sheet name="AccNominee" sheetId="18" r:id="rId12"/>
+    <sheet name="DepoAccBeneficiary" sheetId="21" r:id="rId13"/>
+    <sheet name="EmployeeDetails" sheetId="15" r:id="rId14"/>
+    <sheet name="DefineCreditLine" sheetId="13" r:id="rId15"/>
+    <sheet name="FinProposalRegister" sheetId="14" r:id="rId16"/>
+    <sheet name="FinApproval" sheetId="19" r:id="rId17"/>
+    <sheet name="FinCommitment" sheetId="20" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191028"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="192">
   <si>
     <t>url</t>
   </si>
@@ -552,6 +559,99 @@
   </si>
   <si>
     <t>3111 - Investment Proposal - Data Entry</t>
+  </si>
+  <si>
+    <t>2003 - Scheme Deposit Add / Edit / Inquiry</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>2004 - Deposit Account Nominee</t>
+  </si>
+  <si>
+    <t>nominee_Name</t>
+  </si>
+  <si>
+    <t>father_Name</t>
+  </si>
+  <si>
+    <t>mother_Name</t>
+  </si>
+  <si>
+    <t>Male</t>
+  </si>
+  <si>
+    <t>mailing_Address</t>
+  </si>
+  <si>
+    <t>city</t>
+  </si>
+  <si>
+    <t>share</t>
+  </si>
+  <si>
+    <t>Ramima Begum</t>
+  </si>
+  <si>
+    <t>Abdur Rahim</t>
+  </si>
+  <si>
+    <t>20002545212589600</t>
+  </si>
+  <si>
+    <t>Dhaka</t>
+  </si>
+  <si>
+    <t>Son</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>Abdur Rahaman</t>
+  </si>
+  <si>
+    <t>national_ID</t>
+  </si>
+  <si>
+    <t>BANGLADESH</t>
+  </si>
+  <si>
+    <t>DHAKA</t>
+  </si>
+  <si>
+    <t>approval_Status</t>
+  </si>
+  <si>
+    <t>app_Ref_No</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>testing123</t>
+  </si>
+  <si>
+    <t>3121 - Investment Approval / Sanctions</t>
+  </si>
+  <si>
+    <t>benName</t>
+  </si>
+  <si>
+    <t>benFather</t>
+  </si>
+  <si>
+    <t>benMother</t>
+  </si>
+  <si>
+    <t>20012548789658900</t>
+  </si>
+  <si>
+    <t>2005 - Deposit Account Beneficiary</t>
+  </si>
+  <si>
+    <t>emp-001</t>
   </si>
 </sst>
 </file>
@@ -942,7 +1042,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1001,70 +1101,20 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" display="Ultimus@123" xr:uid="{96BB2AC1-D5EA-49A3-8416-0EEA54340B78}"/>
+    <hyperlink ref="A4" r:id="rId2" xr:uid="{7DCA1D98-5E2B-4662-B2AF-1E3902F43611}"/>
+    <hyperlink ref="A2" r:id="rId3" xr:uid="{784DB843-F097-43D7-BC07-094B9BD07A1A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC147EC4-0543-4D0F-A76B-07552AB7067A}">
-  <dimension ref="A1:E2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2">
-        <v>100000</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52160906-015D-4308-A814-3E4A80805C54}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1097,27 +1147,30 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E24DFEDC-F147-420A-A606-CE8A5A25A847}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -1125,12 +1178,170 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A220D25-A613-44FA-AE19-BCC6EE76ABF8}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" t="s">
+        <v>178</v>
+      </c>
+      <c r="F1" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" t="s">
+        <v>105</v>
+      </c>
+      <c r="H1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" t="s">
+        <v>169</v>
+      </c>
+      <c r="L1" t="s">
+        <v>111</v>
+      </c>
+      <c r="M1" t="s">
+        <v>85</v>
+      </c>
+      <c r="N1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>174</v>
+      </c>
+      <c r="H2" t="s">
+        <v>179</v>
+      </c>
+      <c r="I2" t="s">
+        <v>180</v>
+      </c>
+      <c r="J2" t="s">
+        <v>180</v>
+      </c>
+      <c r="K2" t="s">
+        <v>174</v>
+      </c>
+      <c r="L2" t="s">
+        <v>175</v>
+      </c>
+      <c r="M2" s="9">
+        <v>36841</v>
+      </c>
+      <c r="N2">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A5FF150-DFF6-447C-8A86-E884F10409C8}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>167</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0DE7DD4-3D62-43F3-853A-423D003E7742}">
   <dimension ref="A1:AT2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1296,8 +1507,8 @@
       </c>
     </row>
     <row r="2" spans="1:46" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>996699</v>
+      <c r="A2" t="s">
+        <v>191</v>
       </c>
       <c r="B2" t="s">
         <v>123</v>
@@ -1353,191 +1564,11 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB203C0-CA1F-4DE4-9DFD-626961E733A7}">
-  <dimension ref="A1:C18"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="127.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2">
-        <v>2001</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B3">
-        <v>8002</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4">
-        <v>7031</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5">
-        <v>8001</v>
-      </c>
-      <c r="C5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6">
-        <v>2011</v>
-      </c>
-      <c r="C6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7">
-        <v>2011</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8">
-        <v>7001</v>
-      </c>
-      <c r="C8">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9">
-        <v>2002</v>
-      </c>
-      <c r="C9">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10">
-        <v>2003</v>
-      </c>
-      <c r="C10">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11">
-        <v>1264</v>
-      </c>
-      <c r="C11">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12">
-        <v>3111</v>
-      </c>
-      <c r="C12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="C13">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C14">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C15">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C16">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{571552C5-DA16-4D05-8F28-B75996559A84}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -1614,96 +1645,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B12D6C15-FE60-4052-BA8C-926F90F4933C}">
-  <dimension ref="A1:J13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2">
-        <v>3</v>
-      </c>
-      <c r="E2">
-        <v>100000</v>
-      </c>
-      <c r="F2">
-        <v>12345</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="J13" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D20328DE-E202-43FD-962B-7170F65CDF91}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:V4"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1865,12 +1813,321 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{520352FF-3C64-4147-BA3E-600C45164306}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{553819EE-EFB6-46E5-9349-0EFBBF77EBC3}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CB203C0-CA1F-4DE4-9DFD-626961E733A7}">
+  <dimension ref="A1:C21"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="127.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>2001</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>8002</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4">
+        <v>7031</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5">
+        <v>8001</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6">
+        <v>2011</v>
+      </c>
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7">
+        <v>2011</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8">
+        <v>7001</v>
+      </c>
+      <c r="C8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9">
+        <v>2002</v>
+      </c>
+      <c r="C9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10">
+        <v>2003</v>
+      </c>
+      <c r="C10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>1264</v>
+      </c>
+      <c r="C11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>3111</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13">
+        <v>7032</v>
+      </c>
+      <c r="C13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>2013</v>
+      </c>
+      <c r="C14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>7033</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>2012</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17">
+        <v>2004</v>
+      </c>
+      <c r="C17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18">
+        <v>3121</v>
+      </c>
+      <c r="C18">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>3131</v>
+      </c>
+      <c r="C19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>2005</v>
+      </c>
+      <c r="C20">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E5813B1-5843-40D8-80A2-E35B896B6A5A}">
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1969,21 +2226,23 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08DDB11E-6353-4773-B9C5-3CF2BD55CCEC}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>42</v>
       </c>
@@ -1993,8 +2252,23 @@
       <c r="C1" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
@@ -2003,6 +2277,21 @@
       </c>
       <c r="C2" s="3" t="s">
         <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>15000</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2010,12 +2299,95 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B12D6C15-FE60-4052-BA8C-926F90F4933C}">
+  <dimension ref="A1:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>100000</v>
+      </c>
+      <c r="F2">
+        <v>12345</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="16.5" x14ac:dyDescent="0.3">
+      <c r="J13" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60500C62-56F3-4BCE-B231-A3186E7F6701}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2051,7 +2423,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>161</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -2059,10 +2431,173 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>160</v>
+        <v>38</v>
       </c>
       <c r="B5">
         <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>160</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>163</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>185</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC147EC4-0543-4D0F-A76B-07552AB7067A}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>100000</v>
+      </c>
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD2C5B5-A259-49DA-89E3-9AF6258F1148}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>15000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DD55E16-0765-4584-AA03-D51EA48ACCE6}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>100000</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>